<commit_message>
excel formulas, for Excel 2016
</commit_message>
<xml_diff>
--- a/cheatsheets/xlsx/BehandlungenProKWMitGrunddaten4Excel2016.xlsx
+++ b/cheatsheets/xlsx/BehandlungenProKWMitGrunddaten4Excel2016.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herczeg\Documents\ng2Goodies\cheatsheets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B070A00-EF68-4860-877B-344A4A9F5069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE620B7-0D32-4F0D-94A6-545A693BCC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{10B3320A-F546-4797-AB46-39B2D444BB49}"/>
+    <workbookView xWindow="660" yWindow="450" windowWidth="23700" windowHeight="15885" xr2:uid="{10B3320A-F546-4797-AB46-39B2D444BB49}"/>
   </bookViews>
   <sheets>
     <sheet name="Grunddaten" sheetId="10" r:id="rId1"/>
     <sheet name="KW24" sheetId="16" r:id="rId2"/>
-    <sheet name="KW25" sheetId="20" r:id="rId3"/>
+    <sheet name="KW25" sheetId="21" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,10 +58,10 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={1833554A-8FCF-410A-A4F1-293A2D88A79F}</author>
+    <author>tc={9A86BDE0-3308-444F-BBF4-4DE4FCB7CCF0}</author>
   </authors>
   <commentList>
-    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{1833554A-8FCF-410A-A4F1-293A2D88A79F}">
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{9A86BDE0-3308-444F-BBF4-4DE4FCB7CCF0}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="20">
   <si>
     <t>Frau Mayer</t>
   </si>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>Anzahl Behandlungen diese Woche:</t>
-  </si>
-  <si>
-    <t>Behandelte Personen:</t>
   </si>
   <si>
     <t>Kollege:</t>
@@ -146,19 +143,20 @@
     <t>von der Krankenkasste genehmigte Stunden:</t>
   </si>
   <si>
-    <t>Für diese Person von der KK genehmigte Stunden:</t>
-  </si>
-  <si>
-    <t>Anzahl Behandlungen noch zu planen + machen</t>
-  </si>
-  <si>
-    <t>Anzahl Behandlungen insgesamt gemacht + geplant bis (inkl.) diese Woche:</t>
-  </si>
-  <si>
     <t>Frau Zwei</t>
   </si>
   <si>
     <t>2 St. genehmigt</t>
+  </si>
+  <si>
+    <t>Anzahl Behandlungen noch zu
+planen/machen</t>
+  </si>
+  <si>
+    <t>Anzahl Behandlungen insgesamt gemacht/geplant bis (inkl.) diese Woche:</t>
+  </si>
+  <si>
+    <t>Anzahl Behandlungen noch zu planen/machen</t>
   </si>
 </sst>
 </file>
@@ -166,9 +164,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,12 +226,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -346,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -395,17 +387,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -789,7 +784,7 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="F15" dT="2023-06-05T12:15:23.65" personId="{EB4555AA-DA2A-41A3-9090-9EE073F611C9}" id="{1833554A-8FCF-410A-A4F1-293A2D88A79F}">
+  <threadedComment ref="F15" dT="2023-06-05T12:15:23.65" personId="{EB4555AA-DA2A-41A3-9090-9EE073F611C9}" id="{9A86BDE0-3308-444F-BBF4-4DE4FCB7CCF0}">
     <text>Behandlungen bis zur letzten KW und diese KW zusammen:</text>
   </threadedComment>
 </ThreadedComments>
@@ -799,20 +794,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1522A576-DE82-4FB4-9992-955443B51572}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="22.140625" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>15</v>
+    <row r="1" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -825,7 +820,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="20">
         <v>20</v>
@@ -844,7 +839,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="20">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -854,7 +849,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B7" s="20">
         <v>0</v>
@@ -862,7 +857,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B8" s="20">
         <v>2</v>
@@ -870,7 +865,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="20">
         <v>20</v>
@@ -883,102 +878,105 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0DF0336-157F-455B-9976-2F06187A89F6}">
-  <dimension ref="A1:P55"/>
+  <dimension ref="A1:P64"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
     <col min="13" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23">
+      <c r="B1" s="25">
         <f>MAX(DATE($D$13,1,1),DATE($D$13,1,1)-WEEKDAY(DATE($D$13,1,1),2)+($C$13)*7 + 1)</f>
         <v>45089</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="23">
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="25">
         <f>MAX(DATE($D$13,1,1),DATE($D$13,1,1)-WEEKDAY(DATE($D$13,1,1),2)+($C$13)*7 + 2)</f>
         <v>45090</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="23">
+      <c r="F1" s="25"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="25">
         <f>MAX(DATE($D$13,1,1),DATE($D$13,1,1)-WEEKDAY(DATE($D$13,1,1),2)+($C$13)*7 + 3)</f>
         <v>45091</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="23">
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="25">
         <f>MAX(DATE($D$13,1,1),DATE($D$13,1,1)-WEEKDAY(DATE($D$13,1,1),2)+($C$13)*7 + 4)</f>
         <v>45092</v>
       </c>
-      <c r="L1" s="23"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="23">
+      <c r="L1" s="25"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="25">
         <f>MAX(DATE($D$13,1,1),DATE($D$13,1,1)-WEEKDAY(DATE($D$13,1,1),2)+($C$13)*7 + 5)</f>
         <v>45093</v>
       </c>
-      <c r="O1" s="23"/>
-      <c r="P1" s="24"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="26"/>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="H2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="K2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="N2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1050,7 +1048,7 @@
       <c r="D6" s="9"/>
       <c r="E6" s="11"/>
       <c r="F6" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="8"/>
@@ -1119,11 +1117,13 @@
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="14"/>
+      <c r="H9" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="I9" s="8"/>
       <c r="J9" s="9"/>
       <c r="K9" s="14"/>
@@ -1184,14 +1184,14 @@
       <c r="F12" s="8"/>
       <c r="G12" s="9"/>
       <c r="H12" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="9"/>
       <c r="K12" s="11"/>
       <c r="L12" s="8"/>
       <c r="M12" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N12" s="8"/>
       <c r="O12" s="8"/>
@@ -1199,30 +1199,33 @@
     </row>
     <row r="13" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="19">
         <v>24</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="23">
         <v>2023</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1">
         <f>C13-1</f>
         <v>23</v>
       </c>
-      <c r="M14" s="26"/>
-    </row>
-    <row r="15" spans="1:16" s="12" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="15"/>
+      <c r="M14" s="24"/>
+    </row>
+    <row r="15" spans="1:16" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="str" cm="1">
+        <f t="array" ref="A15:B64">Grunddaten!A1:B50</f>
+        <v>Patient/-in</v>
+      </c>
+      <c r="B15" s="27" t="str">
+        <v>von der Krankenkasste genehmigte Stunden:</v>
+      </c>
       <c r="D15" s="13" t="str">
         <f>"Behandlungen bis (inkl.) KW" &amp; VALUE(C14)</f>
         <v>Behandlungen bis (inkl.) KW23</v>
@@ -1234,82 +1237,80 @@
         <v>18</v>
       </c>
       <c r="G15" s="15"/>
-      <c r="H15" s="13" t="s">
-        <v>16</v>
-      </c>
+      <c r="H15" s="13"/>
       <c r="I15" s="13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B16" t="str" cm="1">
-        <f t="array" ref="B16:B55">Grunddaten!A2:A41</f>
+      <c r="A16" t="str">
         <v>Frau Mayer</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
       </c>
       <c r="C16" s="16">
         <v>1</v>
       </c>
-      <c r="D16" t="e" cm="1">
-        <f t="array" aca="1" ref="D16" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C16 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D16" cm="1">
+        <f t="array" aca="1" ref="D16" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C16 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E16">
-        <f>COUNTIF($B$3:$X$12,B16)</f>
-        <v>1</v>
+        <f>COUNTIF($B$3:$X$12,A16)</f>
+        <v>2</v>
       </c>
       <c r="F16">
         <f ca="1">IFERROR(SUM(D16,E16), E16)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16" s="16"/>
-      <c r="H16">
-        <f>Grunddaten!B2</f>
-        <v>15</v>
-      </c>
       <c r="I16">
-        <f ca="1">H16-F16</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" t="str">
+        <f ca="1">B16-F16</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
         <v>Frau Groß</v>
+      </c>
+      <c r="B17">
+        <v>20</v>
       </c>
       <c r="C17" s="16">
         <v>2</v>
       </c>
-      <c r="D17" t="e" cm="1">
-        <f t="array" aca="1" ref="D17" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C17 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D17" cm="1">
+        <f t="array" aca="1" ref="D17" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C17 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E17">
-        <f t="shared" ref="E17:E49" si="0">COUNTIF($B$3:$X$12,B17)</f>
+        <f t="shared" ref="E17:E49" si="0">COUNTIF($B$3:$X$12,A17)</f>
         <v>1</v>
       </c>
       <c r="F17">
-        <f t="shared" ref="F16:F49" ca="1" si="1">IFERROR(SUM(D17,E17), E17)</f>
+        <f t="shared" ref="F17:F49" ca="1" si="1">IFERROR(SUM(D17,E17), E17)</f>
         <v>1</v>
       </c>
       <c r="G17" s="16"/>
-      <c r="H17">
-        <f>Grunddaten!B3</f>
-        <v>20</v>
-      </c>
       <c r="I17">
-        <f t="shared" ref="I17:I49" ca="1" si="2">H17-F17</f>
+        <f t="shared" ref="I17:I49" ca="1" si="2">B17-F17</f>
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" t="str">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
         <v>Frau Klein</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
       </c>
       <c r="C18" s="16">
         <v>3</v>
       </c>
-      <c r="D18" t="e" cm="1">
-        <f t="array" aca="1" ref="D18" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C18 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D18" cm="1">
+        <f t="array" aca="1" ref="D18" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C18 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
@@ -1320,25 +1321,24 @@
         <v>0</v>
       </c>
       <c r="G18" s="16"/>
-      <c r="H18">
-        <f>Grunddaten!B4</f>
+      <c r="I18">
+        <f t="shared" ca="1" si="2"/>
         <v>15</v>
       </c>
-      <c r="I18">
-        <f t="shared" ca="1" si="2"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" t="str">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
         <v>Frau Rietzinger</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
       </c>
       <c r="C19" s="16">
         <v>4</v>
       </c>
-      <c r="D19" t="e" cm="1">
-        <f t="array" aca="1" ref="D19" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C19 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D19" cm="1">
+        <f t="array" aca="1" ref="D19" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C19 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
@@ -1349,25 +1349,24 @@
         <v>3</v>
       </c>
       <c r="G19" s="16"/>
-      <c r="H19">
-        <f>Grunddaten!B5</f>
-        <v>0</v>
-      </c>
       <c r="I19">
         <f t="shared" ca="1" si="2"/>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" t="str">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
         <v>Frau Schuster</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
       </c>
       <c r="C20" s="16">
         <v>5</v>
       </c>
-      <c r="D20" t="e" cm="1">
-        <f t="array" aca="1" ref="D20" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C20 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D20" cm="1">
+        <f t="array" aca="1" ref="D20" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C20 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
@@ -1378,25 +1377,24 @@
         <v>0</v>
       </c>
       <c r="G20" s="16"/>
-      <c r="H20">
-        <f>Grunddaten!B6</f>
-        <v>0</v>
-      </c>
       <c r="I20">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" t="str">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
         <v>Frau Zwei</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
       </c>
       <c r="C21" s="16">
         <v>6</v>
       </c>
-      <c r="D21" t="e" cm="1">
-        <f t="array" aca="1" ref="D21" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C21 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D21" cm="1">
+        <f t="array" aca="1" ref="D21" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C21 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
@@ -1407,25 +1405,24 @@
         <v>0</v>
       </c>
       <c r="G21" s="16"/>
-      <c r="H21">
-        <f>Grunddaten!B7</f>
-        <v>0</v>
-      </c>
       <c r="I21">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="22" t="str">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
         <v>2 St. genehmigt</v>
+      </c>
+      <c r="B22" s="22">
+        <v>2</v>
       </c>
       <c r="C22" s="16">
         <v>7</v>
       </c>
-      <c r="D22" t="e" cm="1">
-        <f t="array" aca="1" ref="D22" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C22 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D22" cm="1">
+        <f t="array" aca="1" ref="D22" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C22 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
@@ -1436,25 +1433,24 @@
         <v>1</v>
       </c>
       <c r="G22" s="16"/>
-      <c r="H22">
-        <f>Grunddaten!B8</f>
-        <v>2</v>
-      </c>
       <c r="I22">
         <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" t="str">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
         <v>Frau Neu</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
       </c>
       <c r="C23" s="16">
         <v>8</v>
       </c>
-      <c r="D23" t="e" cm="1">
-        <f t="array" aca="1" ref="D23" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C23 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D23" cm="1">
+        <f t="array" aca="1" ref="D23" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C23 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
@@ -1465,25 +1461,24 @@
         <v>2</v>
       </c>
       <c r="G23" s="16"/>
-      <c r="H23">
-        <f>Grunddaten!B9</f>
-        <v>20</v>
-      </c>
       <c r="I23">
         <f t="shared" ca="1" si="2"/>
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0</v>
+      </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24" s="16">
         <v>9</v>
       </c>
-      <c r="D24" t="e" cm="1">
-        <f t="array" aca="1" ref="D24" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C24 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D24" cm="1">
+        <f t="array" aca="1" ref="D24" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C24 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
@@ -1494,25 +1489,24 @@
         <v>0</v>
       </c>
       <c r="G24" s="16"/>
-      <c r="H24">
-        <f>Grunddaten!B10</f>
-        <v>0</v>
-      </c>
       <c r="I24">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0</v>
+      </c>
       <c r="B25">
         <v>0</v>
       </c>
       <c r="C25" s="16">
         <v>10</v>
       </c>
-      <c r="D25" t="e" cm="1">
-        <f t="array" aca="1" ref="D25" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C25 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D25" cm="1">
+        <f t="array" aca="1" ref="D25" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C25 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
@@ -1523,25 +1517,24 @@
         <v>0</v>
       </c>
       <c r="G25" s="16"/>
-      <c r="H25">
-        <f>Grunddaten!B11</f>
-        <v>0</v>
-      </c>
       <c r="I25">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0</v>
+      </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="C26" s="16">
         <v>11</v>
       </c>
-      <c r="D26" t="e" cm="1">
-        <f t="array" aca="1" ref="D26" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C26 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D26" cm="1">
+        <f t="array" aca="1" ref="D26" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C26 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
@@ -1552,25 +1545,24 @@
         <v>0</v>
       </c>
       <c r="G26" s="16"/>
-      <c r="H26">
-        <f>Grunddaten!B12</f>
-        <v>0</v>
-      </c>
       <c r="I26">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27" s="16">
         <v>12</v>
       </c>
-      <c r="D27" t="e" cm="1">
-        <f t="array" aca="1" ref="D27" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C27 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D27" cm="1">
+        <f t="array" aca="1" ref="D27" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C27 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E27">
         <f t="shared" si="0"/>
@@ -1581,25 +1573,24 @@
         <v>0</v>
       </c>
       <c r="G27" s="16"/>
-      <c r="H27">
-        <f>Grunddaten!B13</f>
-        <v>0</v>
-      </c>
       <c r="I27">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
       <c r="B28">
         <v>0</v>
       </c>
       <c r="C28" s="16">
         <v>13</v>
       </c>
-      <c r="D28" t="e" cm="1">
-        <f t="array" aca="1" ref="D28" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C28 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D28" cm="1">
+        <f t="array" aca="1" ref="D28" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C28 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E28">
         <f t="shared" si="0"/>
@@ -1610,25 +1601,24 @@
         <v>0</v>
       </c>
       <c r="G28" s="16"/>
-      <c r="H28">
-        <f>Grunddaten!B14</f>
-        <v>0</v>
-      </c>
       <c r="I28">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0</v>
+      </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="C29" s="16">
         <v>14</v>
       </c>
-      <c r="D29" t="e" cm="1">
-        <f t="array" aca="1" ref="D29" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C29 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D29" cm="1">
+        <f t="array" aca="1" ref="D29" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C29 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E29">
         <f t="shared" si="0"/>
@@ -1639,25 +1629,24 @@
         <v>0</v>
       </c>
       <c r="G29" s="16"/>
-      <c r="H29">
-        <f>Grunddaten!B15</f>
-        <v>0</v>
-      </c>
       <c r="I29">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0</v>
+      </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="C30" s="16">
         <v>15</v>
       </c>
-      <c r="D30" t="e" cm="1">
-        <f t="array" aca="1" ref="D30" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C30 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D30" cm="1">
+        <f t="array" aca="1" ref="D30" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C30 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E30">
         <f t="shared" si="0"/>
@@ -1668,25 +1657,24 @@
         <v>0</v>
       </c>
       <c r="G30" s="16"/>
-      <c r="H30">
-        <f>Grunddaten!B16</f>
-        <v>0</v>
-      </c>
       <c r="I30">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0</v>
+      </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31" s="16">
         <v>16</v>
       </c>
-      <c r="D31" t="e" cm="1">
-        <f t="array" aca="1" ref="D31" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C31 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D31" cm="1">
+        <f t="array" aca="1" ref="D31" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C31 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E31">
         <f t="shared" si="0"/>
@@ -1697,25 +1685,24 @@
         <v>0</v>
       </c>
       <c r="G31" s="16"/>
-      <c r="H31">
-        <f>Grunddaten!B17</f>
-        <v>0</v>
-      </c>
       <c r="I31">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0</v>
+      </c>
       <c r="B32">
         <v>0</v>
       </c>
       <c r="C32" s="16">
         <v>17</v>
       </c>
-      <c r="D32" t="e" cm="1">
-        <f t="array" aca="1" ref="D32" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C32 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D32" cm="1">
+        <f t="array" aca="1" ref="D32" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C32 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E32">
         <f t="shared" si="0"/>
@@ -1726,25 +1713,24 @@
         <v>0</v>
       </c>
       <c r="G32" s="16"/>
-      <c r="H32">
-        <f>Grunddaten!B18</f>
-        <v>0</v>
-      </c>
       <c r="I32">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0</v>
+      </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33" s="16">
         <v>18</v>
       </c>
-      <c r="D33" t="e" cm="1">
-        <f t="array" aca="1" ref="D33" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C33 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D33" cm="1">
+        <f t="array" aca="1" ref="D33" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C33 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E33">
         <f t="shared" si="0"/>
@@ -1755,25 +1741,24 @@
         <v>0</v>
       </c>
       <c r="G33" s="16"/>
-      <c r="H33">
-        <f>Grunddaten!B19</f>
-        <v>0</v>
-      </c>
       <c r="I33">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0</v>
+      </c>
       <c r="B34">
         <v>0</v>
       </c>
       <c r="C34" s="16">
         <v>19</v>
       </c>
-      <c r="D34" t="e" cm="1">
-        <f t="array" aca="1" ref="D34" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C34 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D34" cm="1">
+        <f t="array" aca="1" ref="D34" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C34 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E34">
         <f t="shared" si="0"/>
@@ -1784,25 +1769,24 @@
         <v>0</v>
       </c>
       <c r="G34" s="16"/>
-      <c r="H34">
-        <f>Grunddaten!B20</f>
-        <v>0</v>
-      </c>
       <c r="I34">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0</v>
+      </c>
       <c r="B35">
         <v>0</v>
       </c>
       <c r="C35" s="16">
         <v>20</v>
       </c>
-      <c r="D35" t="e" cm="1">
-        <f t="array" aca="1" ref="D35" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C35 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D35" cm="1">
+        <f t="array" aca="1" ref="D35" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C35 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E35">
         <f t="shared" si="0"/>
@@ -1813,25 +1797,24 @@
         <v>0</v>
       </c>
       <c r="G35" s="16"/>
-      <c r="H35">
-        <f>Grunddaten!B21</f>
-        <v>0</v>
-      </c>
       <c r="I35">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0</v>
+      </c>
       <c r="B36">
         <v>0</v>
       </c>
       <c r="C36" s="16">
         <v>21</v>
       </c>
-      <c r="D36" t="e" cm="1">
-        <f t="array" aca="1" ref="D36" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C36 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D36" cm="1">
+        <f t="array" aca="1" ref="D36" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C36 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E36">
         <f t="shared" si="0"/>
@@ -1842,25 +1825,24 @@
         <v>0</v>
       </c>
       <c r="G36" s="16"/>
-      <c r="H36">
-        <f>Grunddaten!B22</f>
-        <v>0</v>
-      </c>
       <c r="I36">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0</v>
+      </c>
       <c r="B37">
         <v>0</v>
       </c>
       <c r="C37" s="16">
         <v>22</v>
       </c>
-      <c r="D37" t="e" cm="1">
-        <f t="array" aca="1" ref="D37" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C37 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D37" cm="1">
+        <f t="array" aca="1" ref="D37" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C37 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E37">
         <f t="shared" si="0"/>
@@ -1871,25 +1853,24 @@
         <v>0</v>
       </c>
       <c r="G37" s="16"/>
-      <c r="H37">
-        <f>Grunddaten!B23</f>
-        <v>0</v>
-      </c>
       <c r="I37">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>0</v>
+      </c>
       <c r="B38">
         <v>0</v>
       </c>
       <c r="C38" s="16">
         <v>23</v>
       </c>
-      <c r="D38" t="e" cm="1">
-        <f t="array" aca="1" ref="D38" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C38 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D38" cm="1">
+        <f t="array" aca="1" ref="D38" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C38 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E38">
         <f t="shared" si="0"/>
@@ -1900,25 +1881,24 @@
         <v>0</v>
       </c>
       <c r="G38" s="16"/>
-      <c r="H38">
-        <f>Grunddaten!B24</f>
-        <v>0</v>
-      </c>
       <c r="I38">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>0</v>
+      </c>
       <c r="B39">
         <v>0</v>
       </c>
       <c r="C39" s="16">
         <v>24</v>
       </c>
-      <c r="D39" t="e" cm="1">
-        <f t="array" aca="1" ref="D39" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C39 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D39" cm="1">
+        <f t="array" aca="1" ref="D39" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C39 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E39">
         <f t="shared" si="0"/>
@@ -1929,25 +1909,24 @@
         <v>0</v>
       </c>
       <c r="G39" s="16"/>
-      <c r="H39">
-        <f>Grunddaten!B25</f>
-        <v>0</v>
-      </c>
       <c r="I39">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0</v>
+      </c>
       <c r="B40">
         <v>0</v>
       </c>
       <c r="C40" s="16">
         <v>25</v>
       </c>
-      <c r="D40" t="e" cm="1">
-        <f t="array" aca="1" ref="D40" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C40 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D40" cm="1">
+        <f t="array" aca="1" ref="D40" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C40 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E40">
         <f t="shared" si="0"/>
@@ -1958,25 +1937,24 @@
         <v>0</v>
       </c>
       <c r="G40" s="16"/>
-      <c r="H40">
-        <f>Grunddaten!B26</f>
-        <v>0</v>
-      </c>
       <c r="I40">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0</v>
+      </c>
       <c r="B41">
         <v>0</v>
       </c>
       <c r="C41" s="16">
         <v>26</v>
       </c>
-      <c r="D41" t="e" cm="1">
-        <f t="array" aca="1" ref="D41" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C41 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D41" cm="1">
+        <f t="array" aca="1" ref="D41" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C41 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E41">
         <f t="shared" si="0"/>
@@ -1987,25 +1965,24 @@
         <v>0</v>
       </c>
       <c r="G41" s="16"/>
-      <c r="H41">
-        <f>Grunddaten!B27</f>
-        <v>0</v>
-      </c>
       <c r="I41">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0</v>
+      </c>
       <c r="B42">
         <v>0</v>
       </c>
       <c r="C42" s="16">
         <v>27</v>
       </c>
-      <c r="D42" t="e" cm="1">
-        <f t="array" aca="1" ref="D42" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C42 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D42" cm="1">
+        <f t="array" aca="1" ref="D42" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C42 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E42">
         <f t="shared" si="0"/>
@@ -2016,25 +1993,24 @@
         <v>0</v>
       </c>
       <c r="G42" s="16"/>
-      <c r="H42">
-        <f>Grunddaten!B28</f>
-        <v>0</v>
-      </c>
       <c r="I42">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0</v>
+      </c>
       <c r="B43">
         <v>0</v>
       </c>
       <c r="C43" s="16">
         <v>28</v>
       </c>
-      <c r="D43" t="e" cm="1">
-        <f t="array" aca="1" ref="D43" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C43 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D43" cm="1">
+        <f t="array" aca="1" ref="D43" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C43 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E43">
         <f t="shared" si="0"/>
@@ -2045,25 +2021,24 @@
         <v>0</v>
       </c>
       <c r="G43" s="16"/>
-      <c r="H43">
-        <f>Grunddaten!B29</f>
-        <v>0</v>
-      </c>
       <c r="I43">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0</v>
+      </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44" s="16">
         <v>29</v>
       </c>
-      <c r="D44" t="e" cm="1">
-        <f t="array" aca="1" ref="D44" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C44 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D44" cm="1">
+        <f t="array" aca="1" ref="D44" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C44 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E44">
         <f t="shared" si="0"/>
@@ -2074,25 +2049,24 @@
         <v>0</v>
       </c>
       <c r="G44" s="16"/>
-      <c r="H44">
-        <f>Grunddaten!B30</f>
-        <v>0</v>
-      </c>
       <c r="I44">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0</v>
+      </c>
       <c r="B45">
         <v>0</v>
       </c>
       <c r="C45" s="16">
         <v>30</v>
       </c>
-      <c r="D45" t="e" cm="1">
-        <f t="array" aca="1" ref="D45" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C45 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D45" cm="1">
+        <f t="array" aca="1" ref="D45" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C45 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E45">
         <f t="shared" si="0"/>
@@ -2103,25 +2077,24 @@
         <v>0</v>
       </c>
       <c r="G45" s="16"/>
-      <c r="H45">
-        <f>Grunddaten!B31</f>
-        <v>0</v>
-      </c>
       <c r="I45">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>0</v>
+      </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="C46" s="16">
         <v>31</v>
       </c>
-      <c r="D46" t="e" cm="1">
-        <f t="array" aca="1" ref="D46" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C46 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D46" cm="1">
+        <f t="array" aca="1" ref="D46" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C46 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E46">
         <f t="shared" si="0"/>
@@ -2132,25 +2105,24 @@
         <v>0</v>
       </c>
       <c r="G46" s="16"/>
-      <c r="H46">
-        <f>Grunddaten!B32</f>
-        <v>0</v>
-      </c>
       <c r="I46">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>0</v>
+      </c>
       <c r="B47">
         <v>0</v>
       </c>
       <c r="C47" s="16">
         <v>32</v>
       </c>
-      <c r="D47" t="e" cm="1">
-        <f t="array" aca="1" ref="D47" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C47 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D47" cm="1">
+        <f t="array" aca="1" ref="D47" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C47 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E47">
         <f t="shared" si="0"/>
@@ -2161,25 +2133,24 @@
         <v>0</v>
       </c>
       <c r="G47" s="16"/>
-      <c r="H47">
-        <f>Grunddaten!B33</f>
-        <v>0</v>
-      </c>
       <c r="I47">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>0</v>
+      </c>
       <c r="B48">
         <v>0</v>
       </c>
       <c r="C48" s="16">
         <v>33</v>
       </c>
-      <c r="D48" t="e" cm="1">
-        <f t="array" aca="1" ref="D48" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C48 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D48" cm="1">
+        <f t="array" aca="1" ref="D48" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C48 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E48">
         <f t="shared" si="0"/>
@@ -2190,25 +2161,24 @@
         <v>0</v>
       </c>
       <c r="G48" s="16"/>
-      <c r="H48">
-        <f>Grunddaten!B34</f>
-        <v>0</v>
-      </c>
       <c r="I48">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>0</v>
+      </c>
       <c r="B49">
         <v>0</v>
       </c>
       <c r="C49" s="16">
         <v>34</v>
       </c>
-      <c r="D49" t="e" cm="1">
-        <f t="array" aca="1" ref="D49" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C49 + 15,"0"))</f>
-        <v>#REF!</v>
+      <c r="D49" cm="1">
+        <f t="array" aca="1" ref="D49" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C49 + 15,"0")),0)</f>
+        <v>0</v>
       </c>
       <c r="E49">
         <f t="shared" si="0"/>
@@ -2219,50 +2189,136 @@
         <v>0</v>
       </c>
       <c r="G49" s="16"/>
-      <c r="H49">
-        <f>Grunddaten!B35</f>
-        <v>0</v>
-      </c>
       <c r="I49">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>0</v>
+      </c>
       <c r="B50">
         <v>0</v>
       </c>
       <c r="C50" s="16"/>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>0</v>
+      </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="C51" s="16"/>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>0</v>
+      </c>
       <c r="B52">
         <v>0</v>
       </c>
       <c r="C52" s="16"/>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>0</v>
+      </c>
       <c r="B53">
         <v>0</v>
       </c>
       <c r="C53" s="16"/>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>0</v>
+      </c>
       <c r="B54">
         <v>0</v>
       </c>
       <c r="C54" s="16"/>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>0</v>
+      </c>
       <c r="B55">
         <v>0</v>
       </c>
       <c r="C55" s="16"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>0</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>0</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>0</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>0</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>0</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>0</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>0</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>0</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>0</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2290,103 +2346,106 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A37F77E-B26A-44CF-95A1-F379105C98B7}">
-  <dimension ref="A1:P55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D8D5D3-9A3A-4CC1-AFB5-BCD9DDD9868E}">
+  <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
     <col min="13" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23">
+      <c r="B1" s="25">
         <f>MAX(DATE($D$13,1,1),DATE($D$13,1,1)-WEEKDAY(DATE($D$13,1,1),2)+($C$13)*7 + 1)</f>
         <v>45096</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="23">
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="25">
         <f>MAX(DATE($D$13,1,1),DATE($D$13,1,1)-WEEKDAY(DATE($D$13,1,1),2)+($C$13)*7 + 2)</f>
         <v>45097</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="23">
+      <c r="F1" s="25"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="25">
         <f>MAX(DATE($D$13,1,1),DATE($D$13,1,1)-WEEKDAY(DATE($D$13,1,1),2)+($C$13)*7 + 3)</f>
         <v>45098</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="23">
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="25">
         <f>MAX(DATE($D$13,1,1),DATE($D$13,1,1)-WEEKDAY(DATE($D$13,1,1),2)+($C$13)*7 + 4)</f>
         <v>45099</v>
       </c>
-      <c r="L1" s="23"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="23">
+      <c r="L1" s="25"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="25">
         <f>MAX(DATE($D$13,1,1),DATE($D$13,1,1)-WEEKDAY(DATE($D$13,1,1),2)+($C$13)*7 + 5)</f>
         <v>45100</v>
       </c>
-      <c r="O1" s="23"/>
-      <c r="P1" s="24"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="26"/>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="H2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="K2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="N2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -2458,7 +2517,7 @@
       <c r="D6" s="9"/>
       <c r="E6" s="11"/>
       <c r="F6" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="8"/>
@@ -2501,15 +2560,15 @@
       <c r="E8" s="11"/>
       <c r="F8" s="8"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="8"/>
+      <c r="H8" s="8" t="s">
+        <v>2</v>
+      </c>
       <c r="I8" s="8"/>
       <c r="J8" s="9"/>
       <c r="K8" s="11"/>
       <c r="L8" s="8"/>
       <c r="M8" s="9"/>
-      <c r="N8" s="8" t="s">
-        <v>2</v>
-      </c>
+      <c r="N8" s="8"/>
       <c r="O8" s="8"/>
       <c r="P8" s="9"/>
     </row>
@@ -2522,7 +2581,9 @@
         <v>0</v>
       </c>
       <c r="D9" s="9"/>
-      <c r="E9" s="11"/>
+      <c r="E9" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="F9" s="8"/>
       <c r="G9" s="9"/>
       <c r="H9" s="14"/>
@@ -2548,7 +2609,9 @@
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="9"/>
-      <c r="K10" s="11"/>
+      <c r="K10" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="L10" s="8"/>
       <c r="M10" s="9"/>
       <c r="N10" s="8"/>
@@ -2586,14 +2649,14 @@
       <c r="F12" s="8"/>
       <c r="G12" s="9"/>
       <c r="H12" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="9"/>
       <c r="K12" s="11"/>
       <c r="L12" s="8"/>
       <c r="M12" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N12" s="8"/>
       <c r="O12" s="8"/>
@@ -2601,30 +2664,33 @@
     </row>
     <row r="13" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="19">
         <v>25</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="23">
         <v>2023</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1">
         <f>C13-1</f>
         <v>24</v>
       </c>
-      <c r="M14" s="26"/>
-    </row>
-    <row r="15" spans="1:16" s="12" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="15"/>
+      <c r="M14" s="24"/>
+    </row>
+    <row r="15" spans="1:16" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="str" cm="1">
+        <f t="array" ref="A15:B64">Grunddaten!A1:B50</f>
+        <v>Patient/-in</v>
+      </c>
+      <c r="B15" s="27" t="str">
+        <v>von der Krankenkasste genehmigte Stunden:</v>
+      </c>
       <c r="D15" s="13" t="str">
         <f>"Behandlungen bis (inkl.) KW" &amp; VALUE(C14)</f>
         <v>Behandlungen bis (inkl.) KW24</v>
@@ -2636,81 +2702,79 @@
         <v>18</v>
       </c>
       <c r="G15" s="15"/>
-      <c r="H15" s="13" t="s">
-        <v>16</v>
-      </c>
+      <c r="H15" s="13"/>
       <c r="I15" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B16" t="str" cm="1">
-        <f t="array" ref="B16:B55">Grunddaten!A2:A41</f>
+      <c r="A16" t="str">
         <v>Frau Mayer</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
       </c>
       <c r="C16" s="16">
         <v>1</v>
       </c>
       <c r="D16" cm="1">
-        <f t="array" aca="1" ref="D16" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C16 + 15,"0"))</f>
-        <v>1</v>
+        <f t="array" aca="1" ref="D16" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C16 + 15,"0")),0)</f>
+        <v>2</v>
       </c>
       <c r="E16">
-        <f>COUNTIF($B$3:$X$12,B16)</f>
+        <f>COUNTIF($B$3:$X$12,A16)</f>
         <v>1</v>
       </c>
       <c r="F16">
         <f ca="1">IFERROR(SUM(D16,E16), E16)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G16" s="16"/>
-      <c r="H16">
-        <f>Grunddaten!B2</f>
-        <v>15</v>
-      </c>
       <c r="I16">
-        <f ca="1">H16-F16</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" t="str">
+        <f ca="1">B16-F16</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
         <v>Frau Groß</v>
+      </c>
+      <c r="B17">
+        <v>20</v>
       </c>
       <c r="C17" s="16">
         <v>2</v>
       </c>
       <c r="D17" cm="1">
-        <f t="array" aca="1" ref="D17" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C17 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D17" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C17 + 15,"0")),0)</f>
         <v>1</v>
       </c>
       <c r="E17">
-        <f t="shared" ref="E17:E49" si="0">COUNTIF($B$3:$X$12,B17)</f>
-        <v>0</v>
+        <f t="shared" ref="E17:E49" si="0">COUNTIF($B$3:$X$12,A17)</f>
+        <v>1</v>
       </c>
       <c r="F17">
-        <f t="shared" ref="F17:F50" ca="1" si="1">IFERROR(SUM(D17,E17), E17)</f>
-        <v>1</v>
+        <f t="shared" ref="F17:F49" ca="1" si="1">IFERROR(SUM(D17,E17), E17)</f>
+        <v>2</v>
       </c>
       <c r="G17" s="16"/>
-      <c r="H17">
-        <f>Grunddaten!B3</f>
-        <v>20</v>
-      </c>
       <c r="I17">
-        <f t="shared" ref="I17:I49" ca="1" si="2">H17-F17</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" t="str">
+        <f t="shared" ref="I17:I49" ca="1" si="2">B17-F17</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
         <v>Frau Klein</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
       </c>
       <c r="C18" s="16">
         <v>3</v>
       </c>
       <c r="D18" cm="1">
-        <f t="array" aca="1" ref="D18" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C18 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D18" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C18 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E18">
@@ -2722,24 +2786,23 @@
         <v>0</v>
       </c>
       <c r="G18" s="16"/>
-      <c r="H18">
-        <f>Grunddaten!B4</f>
+      <c r="I18">
+        <f t="shared" ca="1" si="2"/>
         <v>15</v>
       </c>
-      <c r="I18">
-        <f t="shared" ca="1" si="2"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" t="str">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
         <v>Frau Rietzinger</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
       </c>
       <c r="C19" s="16">
         <v>4</v>
       </c>
       <c r="D19" cm="1">
-        <f t="array" aca="1" ref="D19" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C19 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D19" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C19 + 15,"0")),0)</f>
         <v>3</v>
       </c>
       <c r="E19">
@@ -2751,53 +2814,51 @@
         <v>4</v>
       </c>
       <c r="G19" s="16"/>
-      <c r="H19">
-        <f>Grunddaten!B5</f>
-        <v>0</v>
-      </c>
       <c r="I19">
         <f t="shared" ca="1" si="2"/>
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
         <v>Frau Schuster</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
       </c>
       <c r="C20" s="16">
         <v>5</v>
       </c>
       <c r="D20" cm="1">
-        <f t="array" aca="1" ref="D20" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C20 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D20" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C20 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="16"/>
-      <c r="H20">
-        <f>Grunddaten!B6</f>
-        <v>0</v>
-      </c>
       <c r="I20">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" t="str">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
         <v>Frau Zwei</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
       </c>
       <c r="C21" s="16">
         <v>6</v>
       </c>
       <c r="D21" cm="1">
-        <f t="array" aca="1" ref="D21" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C21 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D21" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C21 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E21">
@@ -2809,24 +2870,23 @@
         <v>0</v>
       </c>
       <c r="G21" s="16"/>
-      <c r="H21">
-        <f>Grunddaten!B7</f>
-        <v>0</v>
-      </c>
       <c r="I21">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="22" t="str">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
         <v>2 St. genehmigt</v>
+      </c>
+      <c r="B22" s="22">
+        <v>2</v>
       </c>
       <c r="C22" s="16">
         <v>7</v>
       </c>
       <c r="D22" cm="1">
-        <f t="array" aca="1" ref="D22" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C22 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D22" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C22 + 15,"0")),0)</f>
         <v>1</v>
       </c>
       <c r="E22">
@@ -2838,24 +2898,23 @@
         <v>2</v>
       </c>
       <c r="G22" s="16"/>
-      <c r="H22">
-        <f>Grunddaten!B8</f>
-        <v>2</v>
-      </c>
       <c r="I22">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" t="str">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
         <v>Frau Neu</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
       </c>
       <c r="C23" s="16">
         <v>8</v>
       </c>
       <c r="D23" cm="1">
-        <f t="array" aca="1" ref="D23" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C23 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D23" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C23 + 15,"0")),0)</f>
         <v>2</v>
       </c>
       <c r="E23">
@@ -2867,16 +2926,15 @@
         <v>4</v>
       </c>
       <c r="G23" s="16"/>
-      <c r="H23">
-        <f>Grunddaten!B9</f>
-        <v>20</v>
-      </c>
       <c r="I23">
         <f t="shared" ca="1" si="2"/>
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0</v>
+      </c>
       <c r="B24">
         <v>0</v>
       </c>
@@ -2884,7 +2942,7 @@
         <v>9</v>
       </c>
       <c r="D24" cm="1">
-        <f t="array" aca="1" ref="D24" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C24 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D24" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C24 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E24">
@@ -2896,16 +2954,15 @@
         <v>0</v>
       </c>
       <c r="G24" s="16"/>
-      <c r="H24">
-        <f>Grunddaten!B10</f>
-        <v>0</v>
-      </c>
       <c r="I24">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0</v>
+      </c>
       <c r="B25">
         <v>0</v>
       </c>
@@ -2913,7 +2970,7 @@
         <v>10</v>
       </c>
       <c r="D25" cm="1">
-        <f t="array" aca="1" ref="D25" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C25 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D25" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C25 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E25">
@@ -2925,16 +2982,15 @@
         <v>0</v>
       </c>
       <c r="G25" s="16"/>
-      <c r="H25">
-        <f>Grunddaten!B11</f>
-        <v>0</v>
-      </c>
       <c r="I25">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0</v>
+      </c>
       <c r="B26">
         <v>0</v>
       </c>
@@ -2942,7 +2998,7 @@
         <v>11</v>
       </c>
       <c r="D26" cm="1">
-        <f t="array" aca="1" ref="D26" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C26 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D26" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C26 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E26">
@@ -2954,16 +3010,15 @@
         <v>0</v>
       </c>
       <c r="G26" s="16"/>
-      <c r="H26">
-        <f>Grunddaten!B12</f>
-        <v>0</v>
-      </c>
       <c r="I26">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
       <c r="B27">
         <v>0</v>
       </c>
@@ -2971,7 +3026,7 @@
         <v>12</v>
       </c>
       <c r="D27" cm="1">
-        <f t="array" aca="1" ref="D27" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C27 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D27" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C27 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E27">
@@ -2983,16 +3038,15 @@
         <v>0</v>
       </c>
       <c r="G27" s="16"/>
-      <c r="H27">
-        <f>Grunddaten!B13</f>
-        <v>0</v>
-      </c>
       <c r="I27">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
       <c r="B28">
         <v>0</v>
       </c>
@@ -3000,7 +3054,7 @@
         <v>13</v>
       </c>
       <c r="D28" cm="1">
-        <f t="array" aca="1" ref="D28" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C28 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D28" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C28 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E28">
@@ -3012,16 +3066,15 @@
         <v>0</v>
       </c>
       <c r="G28" s="16"/>
-      <c r="H28">
-        <f>Grunddaten!B14</f>
-        <v>0</v>
-      </c>
       <c r="I28">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0</v>
+      </c>
       <c r="B29">
         <v>0</v>
       </c>
@@ -3029,7 +3082,7 @@
         <v>14</v>
       </c>
       <c r="D29" cm="1">
-        <f t="array" aca="1" ref="D29" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C29 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D29" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C29 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E29">
@@ -3041,16 +3094,15 @@
         <v>0</v>
       </c>
       <c r="G29" s="16"/>
-      <c r="H29">
-        <f>Grunddaten!B15</f>
-        <v>0</v>
-      </c>
       <c r="I29">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0</v>
+      </c>
       <c r="B30">
         <v>0</v>
       </c>
@@ -3058,7 +3110,7 @@
         <v>15</v>
       </c>
       <c r="D30" cm="1">
-        <f t="array" aca="1" ref="D30" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C30 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D30" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C30 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E30">
@@ -3070,16 +3122,15 @@
         <v>0</v>
       </c>
       <c r="G30" s="16"/>
-      <c r="H30">
-        <f>Grunddaten!B16</f>
-        <v>0</v>
-      </c>
       <c r="I30">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0</v>
+      </c>
       <c r="B31">
         <v>0</v>
       </c>
@@ -3087,7 +3138,7 @@
         <v>16</v>
       </c>
       <c r="D31" cm="1">
-        <f t="array" aca="1" ref="D31" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C31 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D31" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C31 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E31">
@@ -3099,16 +3150,15 @@
         <v>0</v>
       </c>
       <c r="G31" s="16"/>
-      <c r="H31">
-        <f>Grunddaten!B17</f>
-        <v>0</v>
-      </c>
       <c r="I31">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0</v>
+      </c>
       <c r="B32">
         <v>0</v>
       </c>
@@ -3116,7 +3166,7 @@
         <v>17</v>
       </c>
       <c r="D32" cm="1">
-        <f t="array" aca="1" ref="D32" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C32 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D32" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C32 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E32">
@@ -3128,16 +3178,15 @@
         <v>0</v>
       </c>
       <c r="G32" s="16"/>
-      <c r="H32">
-        <f>Grunddaten!B18</f>
-        <v>0</v>
-      </c>
       <c r="I32">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0</v>
+      </c>
       <c r="B33">
         <v>0</v>
       </c>
@@ -3145,7 +3194,7 @@
         <v>18</v>
       </c>
       <c r="D33" cm="1">
-        <f t="array" aca="1" ref="D33" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C33 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D33" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C33 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E33">
@@ -3157,16 +3206,15 @@
         <v>0</v>
       </c>
       <c r="G33" s="16"/>
-      <c r="H33">
-        <f>Grunddaten!B19</f>
-        <v>0</v>
-      </c>
       <c r="I33">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0</v>
+      </c>
       <c r="B34">
         <v>0</v>
       </c>
@@ -3174,7 +3222,7 @@
         <v>19</v>
       </c>
       <c r="D34" cm="1">
-        <f t="array" aca="1" ref="D34" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C34 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D34" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C34 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E34">
@@ -3186,16 +3234,15 @@
         <v>0</v>
       </c>
       <c r="G34" s="16"/>
-      <c r="H34">
-        <f>Grunddaten!B20</f>
-        <v>0</v>
-      </c>
       <c r="I34">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0</v>
+      </c>
       <c r="B35">
         <v>0</v>
       </c>
@@ -3203,7 +3250,7 @@
         <v>20</v>
       </c>
       <c r="D35" cm="1">
-        <f t="array" aca="1" ref="D35" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C35 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D35" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C35 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E35">
@@ -3215,16 +3262,15 @@
         <v>0</v>
       </c>
       <c r="G35" s="16"/>
-      <c r="H35">
-        <f>Grunddaten!B21</f>
-        <v>0</v>
-      </c>
       <c r="I35">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0</v>
+      </c>
       <c r="B36">
         <v>0</v>
       </c>
@@ -3232,7 +3278,7 @@
         <v>21</v>
       </c>
       <c r="D36" cm="1">
-        <f t="array" aca="1" ref="D36" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C36 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D36" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C36 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E36">
@@ -3244,16 +3290,15 @@
         <v>0</v>
       </c>
       <c r="G36" s="16"/>
-      <c r="H36">
-        <f>Grunddaten!B22</f>
-        <v>0</v>
-      </c>
       <c r="I36">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0</v>
+      </c>
       <c r="B37">
         <v>0</v>
       </c>
@@ -3261,7 +3306,7 @@
         <v>22</v>
       </c>
       <c r="D37" cm="1">
-        <f t="array" aca="1" ref="D37" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C37 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D37" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C37 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E37">
@@ -3273,16 +3318,15 @@
         <v>0</v>
       </c>
       <c r="G37" s="16"/>
-      <c r="H37">
-        <f>Grunddaten!B23</f>
-        <v>0</v>
-      </c>
       <c r="I37">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>0</v>
+      </c>
       <c r="B38">
         <v>0</v>
       </c>
@@ -3290,7 +3334,7 @@
         <v>23</v>
       </c>
       <c r="D38" cm="1">
-        <f t="array" aca="1" ref="D38" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C38 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D38" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C38 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E38">
@@ -3302,16 +3346,15 @@
         <v>0</v>
       </c>
       <c r="G38" s="16"/>
-      <c r="H38">
-        <f>Grunddaten!B24</f>
-        <v>0</v>
-      </c>
       <c r="I38">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>0</v>
+      </c>
       <c r="B39">
         <v>0</v>
       </c>
@@ -3319,7 +3362,7 @@
         <v>24</v>
       </c>
       <c r="D39" cm="1">
-        <f t="array" aca="1" ref="D39" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C39 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D39" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C39 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E39">
@@ -3331,16 +3374,15 @@
         <v>0</v>
       </c>
       <c r="G39" s="16"/>
-      <c r="H39">
-        <f>Grunddaten!B25</f>
-        <v>0</v>
-      </c>
       <c r="I39">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0</v>
+      </c>
       <c r="B40">
         <v>0</v>
       </c>
@@ -3348,7 +3390,7 @@
         <v>25</v>
       </c>
       <c r="D40" cm="1">
-        <f t="array" aca="1" ref="D40" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C40 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D40" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C40 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E40">
@@ -3360,16 +3402,15 @@
         <v>0</v>
       </c>
       <c r="G40" s="16"/>
-      <c r="H40">
-        <f>Grunddaten!B26</f>
-        <v>0</v>
-      </c>
       <c r="I40">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0</v>
+      </c>
       <c r="B41">
         <v>0</v>
       </c>
@@ -3377,7 +3418,7 @@
         <v>26</v>
       </c>
       <c r="D41" cm="1">
-        <f t="array" aca="1" ref="D41" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C41 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D41" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C41 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E41">
@@ -3389,16 +3430,15 @@
         <v>0</v>
       </c>
       <c r="G41" s="16"/>
-      <c r="H41">
-        <f>Grunddaten!B27</f>
-        <v>0</v>
-      </c>
       <c r="I41">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0</v>
+      </c>
       <c r="B42">
         <v>0</v>
       </c>
@@ -3406,7 +3446,7 @@
         <v>27</v>
       </c>
       <c r="D42" cm="1">
-        <f t="array" aca="1" ref="D42" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C42 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D42" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C42 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E42">
@@ -3418,16 +3458,15 @@
         <v>0</v>
       </c>
       <c r="G42" s="16"/>
-      <c r="H42">
-        <f>Grunddaten!B28</f>
-        <v>0</v>
-      </c>
       <c r="I42">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0</v>
+      </c>
       <c r="B43">
         <v>0</v>
       </c>
@@ -3435,7 +3474,7 @@
         <v>28</v>
       </c>
       <c r="D43" cm="1">
-        <f t="array" aca="1" ref="D43" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C43 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D43" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C43 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E43">
@@ -3447,16 +3486,15 @@
         <v>0</v>
       </c>
       <c r="G43" s="16"/>
-      <c r="H43">
-        <f>Grunddaten!B29</f>
-        <v>0</v>
-      </c>
       <c r="I43">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0</v>
+      </c>
       <c r="B44">
         <v>0</v>
       </c>
@@ -3464,7 +3502,7 @@
         <v>29</v>
       </c>
       <c r="D44" cm="1">
-        <f t="array" aca="1" ref="D44" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C44 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D44" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C44 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E44">
@@ -3476,16 +3514,15 @@
         <v>0</v>
       </c>
       <c r="G44" s="16"/>
-      <c r="H44">
-        <f>Grunddaten!B30</f>
-        <v>0</v>
-      </c>
       <c r="I44">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0</v>
+      </c>
       <c r="B45">
         <v>0</v>
       </c>
@@ -3493,7 +3530,7 @@
         <v>30</v>
       </c>
       <c r="D45" cm="1">
-        <f t="array" aca="1" ref="D45" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C45 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D45" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C45 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E45">
@@ -3505,16 +3542,15 @@
         <v>0</v>
       </c>
       <c r="G45" s="16"/>
-      <c r="H45">
-        <f>Grunddaten!B31</f>
-        <v>0</v>
-      </c>
       <c r="I45">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>0</v>
+      </c>
       <c r="B46">
         <v>0</v>
       </c>
@@ -3522,7 +3558,7 @@
         <v>31</v>
       </c>
       <c r="D46" cm="1">
-        <f t="array" aca="1" ref="D46" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C46 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D46" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C46 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E46">
@@ -3534,16 +3570,15 @@
         <v>0</v>
       </c>
       <c r="G46" s="16"/>
-      <c r="H46">
-        <f>Grunddaten!B32</f>
-        <v>0</v>
-      </c>
       <c r="I46">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>0</v>
+      </c>
       <c r="B47">
         <v>0</v>
       </c>
@@ -3551,7 +3586,7 @@
         <v>32</v>
       </c>
       <c r="D47" cm="1">
-        <f t="array" aca="1" ref="D47" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C47 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D47" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C47 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E47">
@@ -3563,16 +3598,15 @@
         <v>0</v>
       </c>
       <c r="G47" s="16"/>
-      <c r="H47">
-        <f>Grunddaten!B33</f>
-        <v>0</v>
-      </c>
       <c r="I47">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>0</v>
+      </c>
       <c r="B48">
         <v>0</v>
       </c>
@@ -3580,7 +3614,7 @@
         <v>33</v>
       </c>
       <c r="D48" cm="1">
-        <f t="array" aca="1" ref="D48" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C48 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D48" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C48 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E48">
@@ -3592,16 +3626,15 @@
         <v>0</v>
       </c>
       <c r="G48" s="16"/>
-      <c r="H48">
-        <f>Grunddaten!B34</f>
-        <v>0</v>
-      </c>
       <c r="I48">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>0</v>
+      </c>
       <c r="B49">
         <v>0</v>
       </c>
@@ -3609,7 +3642,7 @@
         <v>34</v>
       </c>
       <c r="D49" cm="1">
-        <f t="array" aca="1" ref="D49" ca="1">INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C49 + 15,"0"))</f>
+        <f t="array" aca="1" ref="D49" ca="1">IFERROR(INDIRECT("KW"&amp;VALUE($C$14)&amp;"!F" &amp; TEXT(C49 + 15,"0")),0)</f>
         <v>0</v>
       </c>
       <c r="E49">
@@ -3621,50 +3654,136 @@
         <v>0</v>
       </c>
       <c r="G49" s="16"/>
-      <c r="H49">
-        <f>Grunddaten!B35</f>
-        <v>0</v>
-      </c>
       <c r="I49">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>0</v>
+      </c>
       <c r="B50">
         <v>0</v>
       </c>
       <c r="C50" s="16"/>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>0</v>
+      </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="C51" s="16"/>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>0</v>
+      </c>
       <c r="B52">
         <v>0</v>
       </c>
       <c r="C52" s="16"/>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>0</v>
+      </c>
       <c r="B53">
         <v>0</v>
       </c>
       <c r="C53" s="16"/>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>0</v>
+      </c>
       <c r="B54">
         <v>0</v>
       </c>
       <c r="C54" s="16"/>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>0</v>
+      </c>
       <c r="B55">
         <v>0</v>
       </c>
       <c r="C55" s="16"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>0</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>0</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>0</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>0</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>0</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>0</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>0</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>0</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>0</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
excel formulas converted to Open Office Calc (*.ods)
</commit_message>
<xml_diff>
--- a/cheatsheets/xlsx/BehandlungenProKWMitGrunddaten4Excel2016.xlsx
+++ b/cheatsheets/xlsx/BehandlungenProKWMitGrunddaten4Excel2016.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herczeg\Documents\ng2Goodies\cheatsheets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D60321A-D299-40F0-9E6A-E8047B1A4C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E38F69-85FC-4021-8EE5-BB05ECC44B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="450" windowWidth="23700" windowHeight="15885" activeTab="2" xr2:uid="{10B3320A-F546-4797-AB46-39B2D444BB49}"/>
+    <workbookView xWindow="-26115" yWindow="450" windowWidth="23700" windowHeight="15885" xr2:uid="{10B3320A-F546-4797-AB46-39B2D444BB49}"/>
   </bookViews>
   <sheets>
     <sheet name="Grunddaten" sheetId="10" r:id="rId1"/>
@@ -140,9 +140,6 @@
     <t>Aktuelle KW:</t>
   </si>
   <si>
-    <t>von der Krankenkasste genehmigte Stunden:</t>
-  </si>
-  <si>
     <t>Frau Zwei</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>Anzahl Behandlungen noch zu planen/machen</t>
+  </si>
+  <si>
+    <t>von der Krankenkasse genehmigte Stunden:</t>
   </si>
 </sst>
 </file>
@@ -788,7 +788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1522A576-DE82-4FB4-9992-955443B51572}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -801,7 +801,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -843,7 +843,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="20">
         <v>0</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="20">
         <v>2</v>
@@ -1042,7 +1042,7 @@
       <c r="D6" s="9"/>
       <c r="E6" s="11"/>
       <c r="F6" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="8"/>
@@ -1218,7 +1218,7 @@
         <v>Patient/-in</v>
       </c>
       <c r="B15" s="25" t="str">
-        <v>von der Krankenkasste genehmigte Stunden:</v>
+        <v>von der Krankenkasse genehmigte Stunden:</v>
       </c>
       <c r="D15" s="13" t="str">
         <f>"Behandlungen bis (inkl.) KW" &amp; VALUE(C14)</f>
@@ -1228,12 +1228,12 @@
         <v>4</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -2343,7 +2343,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D8D5D3-9A3A-4CC1-AFB5-BCD9DDD9868E}">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2511,7 +2513,7 @@
       <c r="D6" s="9"/>
       <c r="E6" s="11"/>
       <c r="F6" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="8"/>
@@ -2683,7 +2685,7 @@
         <v>Patient/-in</v>
       </c>
       <c r="B15" s="25" t="str">
-        <v>von der Krankenkasste genehmigte Stunden:</v>
+        <v>von der Krankenkasse genehmigte Stunden:</v>
       </c>
       <c r="D15" s="13" t="str">
         <f>"Behandlungen bis (inkl.) KW" &amp; VALUE(C14)</f>
@@ -2693,12 +2695,12 @@
         <v>4</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FAQ page for working with the Excel file
</commit_message>
<xml_diff>
--- a/cheatsheets/xlsx/BehandlungenProKWMitGrunddaten4Excel2016.xlsx
+++ b/cheatsheets/xlsx/BehandlungenProKWMitGrunddaten4Excel2016.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herczeg\Documents\ng2Goodies\cheatsheets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E38F69-85FC-4021-8EE5-BB05ECC44B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DF2B19-C8AE-4991-A8C9-00C5BAEA1D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26115" yWindow="450" windowWidth="23700" windowHeight="15885" xr2:uid="{10B3320A-F546-4797-AB46-39B2D444BB49}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{10B3320A-F546-4797-AB46-39B2D444BB49}"/>
   </bookViews>
   <sheets>
     <sheet name="Grunddaten" sheetId="10" r:id="rId1"/>
-    <sheet name="KW24" sheetId="16" r:id="rId2"/>
-    <sheet name="KW25" sheetId="21" r:id="rId3"/>
+    <sheet name="FAQ" sheetId="22" r:id="rId2"/>
+    <sheet name="KW24" sheetId="16" r:id="rId3"/>
+    <sheet name="KW25" sheetId="21" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="28">
   <si>
     <t>Frau Mayer</t>
   </si>
@@ -158,6 +159,243 @@
   <si>
     <t>von der Krankenkasse genehmigte Stunden:</t>
   </si>
+  <si>
+    <t>Wie gebe ich bereits in der Vergangenheit (=vor der ersten hier erfassten KW) erfolgte Behandlungen ein?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3 Wochen nach Abschluss der Behandlung kann der "abgeschlossene" Patient aus den Grunddaten entfernt werden:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rechte Maustaste -&gt; "Zellen löschen"</t>
+    </r>
+  </si>
+  <si>
+    <t>1. auszudruckenden Bereich mit der Maus selektieren
+(siehe rechts auf dem 1. Bild)
+2. Datei drucken -&gt; Nur Auswahl, Querformat, Blatt auf einer Seite</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Rechte Maustaste auf letzte/aktuellste Lasche -&gt;
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Verschieben oder Kopieren"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2. im angezeigten Dialog </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"ans Ende stellen"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> und </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Kopie Erstellen"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> aktivieren
+3. die so neu angelegte Lasche richtig benennen: zB. KW29
+4. in Zelle mit </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rotem</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Hintergrund die richtige Kalenderwoche eintragen
+5. Zellen mit Behandlungsterminen der Woche (=hellgrüner Bereich) markieren -&gt; Rechte Maustaste -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Inhalte löschen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+6. Namen für die neuen Behandlungstermine eingeben (am besten via </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Text-Kopie aus den Grunddaten</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, damit der Text ganz sicher gleich bleibt!)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wann kann ich einen Patienten, dessen Behandlung abgeschlossen ist, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>löschen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wie </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>drucke</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ich den Behandlungsplan der aktuellen Woche aus?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wie erstelle ich eine Lasche für eine </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>neue KW</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <t>In Lasche mit der KW, die die Vergangenheit repräsentiert,
+In der Spalte F kann man die hinterlegte Formel durch feste Werte ersetzen.</t>
+  </si>
 </sst>
 </file>
 
@@ -166,7 +404,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,8 +471,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,6 +554,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEFBD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFABE9FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8C7F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -332,7 +603,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -395,6 +666,21 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -456,6 +742,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF8C7F9"/>
+      <color rgb="FFABE9FF"/>
+      <color rgb="FFE1F2CE"/>
+      <color rgb="FFFFEFBD"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -465,6 +759,133 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3914775</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>570294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>674525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D54BE66-1AE3-85BD-B2ED-16E06F35D328}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7058025" y="570294"/>
+          <a:ext cx="2600325" cy="1437731"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>407692</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>665381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DD97988-A7C9-93A2-7BEE-D25BC7C94A2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9761242" y="571500"/>
+          <a:ext cx="3145133" cy="1427381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -788,7 +1209,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1522A576-DE82-4FB4-9992-955443B51572}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -871,10 +1294,156 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8494114E-92F1-4154-8A15-42F205562E4B}">
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="47.140625" customWidth="1"/>
+    <col min="2" max="2" width="58.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="28"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="28"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="28"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="28"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="28"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="28"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="28"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="28"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="28"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="28"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="28"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0DF0336-157F-455B-9976-2F06187A89F6}">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2339,12 +2908,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D8D5D3-9A3A-4CC1-AFB5-BCD9DDD9868E}">
-  <dimension ref="A1:P64"/>
+  <dimension ref="A1:S64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2362,7 +2931,7 @@
     <col min="19" max="20" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="26">
         <f>MAX(DATE($D$13,1,1),DATE($D$13,1,1)-WEEKDAY(DATE($D$13,1,1),2)+($C$13)*7 + 1)</f>
         <v>45096</v>
@@ -2393,58 +2962,73 @@
       </c>
       <c r="O1" s="26"/>
       <c r="P1" s="27"/>
-    </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q1" s="26">
+        <f t="shared" ref="Q1" si="3">N1+1</f>
+        <v>45101</v>
+      </c>
+      <c r="R1" s="26"/>
+      <c r="S1" s="27"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="31" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" s="31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0.33333333333333331</v>
       </c>
@@ -2463,8 +3047,11 @@
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
       <c r="P3" s="9"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="9"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0.375</v>
       </c>
@@ -2483,8 +3070,11 @@
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
       <c r="P4" s="9"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="9"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>0.41666666666666702</v>
       </c>
@@ -2503,8 +3093,11 @@
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
       <c r="P5" s="9"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="9"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>0.45833333333333298</v>
       </c>
@@ -2525,8 +3118,11 @@
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
       <c r="P6" s="9"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="9"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>0.5</v>
       </c>
@@ -2545,8 +3141,11 @@
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
       <c r="P7" s="9"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="9"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>0.54166666666666696</v>
       </c>
@@ -2567,8 +3166,11 @@
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
       <c r="P8" s="9"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="9"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>0.58333333333333304</v>
       </c>
@@ -2591,8 +3193,11 @@
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
       <c r="P9" s="9"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="9"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>0.625</v>
       </c>
@@ -2613,8 +3218,11 @@
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
       <c r="P10" s="9"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="9"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>0.66666666666666696</v>
       </c>
@@ -2633,8 +3241,11 @@
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
       <c r="P11" s="9"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="9"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>0.70833333333333304</v>
       </c>
@@ -2657,8 +3268,11 @@
       <c r="N12" s="8"/>
       <c r="O12" s="8"/>
       <c r="P12" s="9"/>
-    </row>
-    <row r="13" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="9"/>
+    </row>
+    <row r="13" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="21" t="s">
         <v>13</v>
       </c>
@@ -2669,7 +3283,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2679,7 +3293,7 @@
       </c>
       <c r="M14" s="24"/>
     </row>
-    <row r="15" spans="1:16" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="str" cm="1">
         <f t="array" ref="A15:B64">Grunddaten!A1:B50</f>
         <v>Patient/-in</v>
@@ -2703,7 +3317,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <v>Frau Mayer</v>
       </c>
@@ -2746,16 +3360,16 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <f t="shared" ref="E17:E49" si="3">COUNTIF($B$3:$X$12,A17)</f>
+        <f t="shared" ref="E17:E49" si="4">COUNTIF($B$3:$X$12,A17)</f>
         <v>1</v>
       </c>
       <c r="F17">
-        <f t="shared" ref="F17:F49" ca="1" si="4">IFERROR(SUM(D17,E17), E17)</f>
+        <f t="shared" ref="F17:F49" ca="1" si="5">IFERROR(SUM(D17,E17), E17)</f>
         <v>2</v>
       </c>
       <c r="G17" s="16"/>
       <c r="I17">
-        <f t="shared" ref="I17:I49" ca="1" si="5">B17-F17</f>
+        <f t="shared" ref="I17:I49" ca="1" si="6">B17-F17</f>
         <v>18</v>
       </c>
     </row>
@@ -2774,16 +3388,16 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F18">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G18" s="16"/>
       <c r="I18">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>15</v>
       </c>
     </row>
@@ -2802,16 +3416,16 @@
         <v>3</v>
       </c>
       <c r="E19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F19">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>4</v>
       </c>
       <c r="G19" s="16"/>
       <c r="I19">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -2830,16 +3444,16 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F20">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>1</v>
       </c>
       <c r="G20" s="16"/>
       <c r="I20">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>-1</v>
       </c>
     </row>
@@ -2858,16 +3472,16 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F21">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G21" s="16"/>
       <c r="I21">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2886,16 +3500,16 @@
         <v>1</v>
       </c>
       <c r="E22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F22">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2</v>
       </c>
       <c r="G22" s="16"/>
       <c r="I22">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2914,16 +3528,16 @@
         <v>2</v>
       </c>
       <c r="E23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="F23">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>4</v>
       </c>
       <c r="G23" s="16"/>
       <c r="I23">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>16</v>
       </c>
     </row>
@@ -2942,16 +3556,16 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F24">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G24" s="16"/>
       <c r="I24">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2970,16 +3584,16 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F25">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G25" s="16"/>
       <c r="I25">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2998,16 +3612,16 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F26">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G26" s="16"/>
       <c r="I26">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3026,16 +3640,16 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F27">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G27" s="16"/>
       <c r="I27">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3054,16 +3668,16 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F28">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G28" s="16"/>
       <c r="I28">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3082,16 +3696,16 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F29">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G29" s="16"/>
       <c r="I29">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3110,16 +3724,16 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F30">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G30" s="16"/>
       <c r="I30">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3138,16 +3752,16 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F31">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G31" s="16"/>
       <c r="I31">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3166,16 +3780,16 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F32">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G32" s="16"/>
       <c r="I32">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3194,16 +3808,16 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F33">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G33" s="16"/>
       <c r="I33">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3222,16 +3836,16 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F34">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G34" s="16"/>
       <c r="I34">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3250,16 +3864,16 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F35">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G35" s="16"/>
       <c r="I35">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3278,16 +3892,16 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F36">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G36" s="16"/>
       <c r="I36">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3306,16 +3920,16 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F37">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G37" s="16"/>
       <c r="I37">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3334,16 +3948,16 @@
         <v>0</v>
       </c>
       <c r="E38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F38">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G38" s="16"/>
       <c r="I38">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3362,16 +3976,16 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F39">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G39" s="16"/>
       <c r="I39">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3390,16 +4004,16 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F40">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G40" s="16"/>
       <c r="I40">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3418,16 +4032,16 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F41">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G41" s="16"/>
       <c r="I41">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3446,16 +4060,16 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F42">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G42" s="16"/>
       <c r="I42">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3474,16 +4088,16 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F43">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G43" s="16"/>
       <c r="I43">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3502,16 +4116,16 @@
         <v>0</v>
       </c>
       <c r="E44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F44">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G44" s="16"/>
       <c r="I44">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3530,16 +4144,16 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F45">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G45" s="16"/>
       <c r="I45">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3558,16 +4172,16 @@
         <v>0</v>
       </c>
       <c r="E46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F46">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G46" s="16"/>
       <c r="I46">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3586,16 +4200,16 @@
         <v>0</v>
       </c>
       <c r="E47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F47">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G47" s="16"/>
       <c r="I47">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3614,16 +4228,16 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F48">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G48" s="16"/>
       <c r="I48">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3642,16 +4256,16 @@
         <v>0</v>
       </c>
       <c r="E49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F49">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G49" s="16"/>
       <c r="I49">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3782,7 +4396,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>

</xml_diff>